<commit_message>
passed genounce, trying to go-publish
</commit_message>
<xml_diff>
--- a/output/CodeSystem-meuhedet-lab-result-code.xlsx
+++ b/output/CodeSystem-meuhedet-lab-result-code.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>0.1.0</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-03T08:59:15+02:00</t>
+    <t>2024-03-03T10:40:33+02:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>

<commit_message>
corrected all sorts of errors
</commit_message>
<xml_diff>
--- a/output/CodeSystem-meuhedet-lab-result-code.xlsx
+++ b/output/CodeSystem-meuhedet-lab-result-code.xlsx
@@ -24,7 +24,7 @@
     <t>URL</t>
   </si>
   <si>
-    <t>http://fhir.meuhedet.co.il/code/lab-result</t>
+    <t>http://ig.fhir-il-community.org/LRC/CodeSystem/meuhedet-lab-result-code</t>
   </si>
   <si>
     <t>Version</t>
@@ -60,13 +60,13 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-03-03T10:40:33+02:00</t>
+    <t>2024-03-04T15:01:53+02:00</t>
   </si>
   <si>
     <t>Publisher</t>
   </si>
   <si>
-    <t>Outburn LTD.</t>
+    <t>FHIR-il community</t>
   </si>
   <si>
     <t>Contact</t>
@@ -105,7 +105,7 @@
     <t>Content</t>
   </si>
   <si>
-    <t>fragment</t>
+    <t>complete</t>
   </si>
   <si>
     <t>Supplements</t>

</xml_diff>